<commit_message>
Added alliance level and army bonuses
</commit_message>
<xml_diff>
--- a/src/faction_data.xlsx
+++ b/src/faction_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC028114-A5B8-443B-90F9-8A252949585C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADEAED8-52FA-4E07-A812-3B0EA93C629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Mordor</t>
   </si>
   <si>
-    <t>&lt;b&gt;"Our Enemy is Ready, His full Strength gathered"&lt;/b&gt; - Whilst you have more models on the board than your opponent, friendly Mordor Warrior models gain + 1 Courage and may re-roll ls To Wound when making Strikes.</t>
-  </si>
-  <si>
     <t>['The Easterlings', 'The Serpent Horde']</t>
   </si>
   <si>
@@ -187,13 +184,6 @@
   </si>
   <si>
     <t>The Return of the King</t>
-  </si>
-  <si>
-    <t>Barad Dur</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;"The Power of the Ring Could not be Undone"&lt;/b&gt; - Sauron's warband size is increased to 24. Additionally, a force that contains solely of models from the Barad-dûr army list will never be considered Broken if Sauron has 3 or more Wounds remaining. 
- Should Sauron have 2 or fewer Wounds remaining, the army will break as normal. Should Sauron be slain, the army will immediately count as being Broken.</t>
   </si>
   <si>
     <t>['Desolator of the North']</t>
@@ -556,9 +546,6 @@
   <si>
     <t>&lt;b&gt;"Ride for Ruin and the World's Ending!"&lt;/b&gt; - Friendly Rohan Cavalry models gain +1 Strength on a turn in which they Charge.
 &lt;b&gt;"Death!"&lt;/b&gt; - Once per game, at the start of any Fight phase, so long as he is alive and on the battlefield, Théoden can declare that he is using this ability. Every friendly Rohan Hero within 12" may declare either a Heroic Combat or Heroic Strike (if able without expending Might points to do so.</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;"You have my sword."&lt;/b&gt; - Friendly As long as Frodo is alive and on the table (or escapes the board in Scenarios where this applies), all models from The Fellowship army list gain the Fearless special rule. Additionally, a force that consists solely of models from The Fellowship army list will never be considered broken if Frodo is alive and on the table (or escapes the board in Scenarios where this applies).</t>
   </si>
   <si>
     <t>&lt;b&gt;"They're dangerous folk, wandering the wilds"&lt;/b&gt; - All models from this army list gain the Woodland Creature special rule, and the Rangers of the North and Dunedain may benefit from the Stand Fast! of Arathorn, Halbarad and Aragorn - Strider. Additionally, the Rangers of the North and the Dunedain increase their Attacks value to 2, while they have the Infantry keyword.</t>
@@ -839,6 +826,18 @@
     <t>&lt;b&gt;"No quarter was asked..."&lt;/b&gt; - Easterling models receive +1 Courage when their force is Broken. Additionally, once per game, in Scenarios in which a die is rolled to see when the game ends, so long as there is at least one Easterling Hero model alive and on the battlefield, the Easterling player may choose to have the dice re-rolled if the Scenario ends before they wish it to.
 &lt;b&gt;"The Dragon Cults"&lt;/b&gt; - Easterling Warriors and Easterling Kataphrakts in warbands led by the Dragon Emperor or Easterling Dragon Knights do not need to pay the points to be upgraded to Black Dragons - this upgrade is free.
 &lt;b&gt;"Heroes of the Easterlings"&lt;/b&gt; - Easterling Hero models may re-roll a D6 in a Duel roll.</t>
+  </si>
+  <si>
+    <t>Barad-dur</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;"The Power of the Ring Could not be Undone"&lt;/b&gt; - Sauron's warband size is increased to 24. Additionally, a force that contains solely of models from the Barad-dûr army list will never be considered Broken if Sauron has 3 or more Wounds remaining. Should Sauron have 2 or fewer Wounds remaining, the army will break as normal. Should Sauron be slain, the army will immediately count as being Broken.</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;"You have my sword."&lt;/b&gt; - As long as Frodo is alive and on the table (or escapes the board in Scenarios where this applies), all models from The Fellowship army list gain the Fearless special rule. Additionally, a force that consists solely of models from The Fellowship army list will never be considered broken if Frodo is alive and on the table (or escapes the board in Scenarios where this applies).</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;"Our Enemy is Ready, His full Strength gathered"&lt;/b&gt; - Whilst you have more models on the board than your opponent, friendly Mordor Warrior models gain + 1 Courage and may re-roll 1s To Wound when making Strikes.</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,942 +1250,943 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="285" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>225</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>226</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" ht="375" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" ht="300" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="300" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="315" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" ht="285" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" ht="390" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" ht="405" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>